<commit_message>
Updates of shocks, databases and codes
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Interventions/Biomass_ongrid.xlsx
+++ b/CVX_Kenya/Interventions/Biomass_ongrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Interventions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A99E35-3892-431F-9C4A-45869B731638}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6310E5E7-FC8C-4981-93D2-308607DA2608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="260">
   <si>
     <t>level_row</t>
   </si>
@@ -577,9 +577,6 @@
     <t>kSh</t>
   </si>
   <si>
-    <t>Efficiency of the machine</t>
-  </si>
-  <si>
     <t>Heating value petroleum</t>
   </si>
   <si>
@@ -721,9 +718,6 @@
     <t>Value of avoided fertilizer N</t>
   </si>
   <si>
-    <t>Transport increase</t>
-  </si>
-  <si>
     <t>Number of GenSets</t>
   </si>
   <si>
@@ -802,19 +796,37 @@
     <t xml:space="preserve">Decrease in use of Petroleum </t>
   </si>
   <si>
-    <t>Public electricity and heat production</t>
-  </si>
-  <si>
     <t>Decrease in the use of Fertilzers N</t>
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Electricity and Heat</t>
+  </si>
+  <si>
+    <t>Public electricity and heat production CO2 emissions</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>JRC SAM + EORA @2014 (own elaboration)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,7 +1021,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1076,9 +1088,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1087,13 +1096,13 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1106,6 +1115,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1425,7 +1441,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,7 +1450,8 @@
     <col min="2" max="2" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1456,17 +1473,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
         <v>122</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
       <c r="E2" s="33">
         <f>main!C35</f>
-        <v>-54</v>
+        <v>-2.5592417061611375E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1601,7 +1618,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1621,14 +1638,14 @@
         <v>122</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G2" s="5">
         <f>main!C32</f>
         <v>-2053.375196232339</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1648,14 +1665,14 @@
         <v>91</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G3" s="43">
+        <v>190</v>
+      </c>
+      <c r="G3" s="40">
         <f>main!C33</f>
-        <v>-1275.5999999999999</v>
+        <v>-1417.3333333333333</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1738,7 +1755,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1755,14 +1772,14 @@
         <v>122</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F2" s="33">
         <f>main!C34</f>
         <v>216.852</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2469,8 +2486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2495,7 +2512,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>173</v>
@@ -2508,212 +2525,218 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
+      <c r="A2" s="46"/>
       <c r="B2" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="24">
         <v>10000</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
+      <c r="A3" s="46"/>
       <c r="B3" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="41">
+        <v>202</v>
+      </c>
+      <c r="C3" s="48">
+        <f>C20</f>
         <v>0</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="24">
         <v>500</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="37" t="s">
-        <v>251</v>
+      <c r="A5" s="46"/>
+      <c r="B5" s="36" t="s">
+        <v>249</v>
       </c>
       <c r="C5" s="24">
         <v>80</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" s="40">
+      <c r="A6" s="46"/>
+      <c r="B6" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" s="39">
+        <f>0.27</f>
         <v>0.27</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="37" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="46"/>
+      <c r="B7" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="C7" s="39">
+        <v>2110</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="47"/>
-      <c r="B7" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="24">
+      <c r="F7" s="18"/>
+      <c r="G7" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="46"/>
+      <c r="B8" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="24">
         <v>0.4</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="47"/>
-      <c r="B8" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="24">
-        <v>106.3</v>
-      </c>
       <c r="D8" s="24"/>
-      <c r="E8" s="24" t="s">
-        <v>212</v>
-      </c>
+      <c r="E8" s="24"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="17" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="C9" s="24">
-        <v>39</v>
+        <v>106.3</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="F9" s="18"/>
-      <c r="G9" s="18" t="s">
-        <v>252</v>
-      </c>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C10" s="24">
-        <v>0.98</v>
+        <v>39</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="47"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C11" s="24">
-        <v>0.109</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>196</v>
-      </c>
+        <v>0.98</v>
+      </c>
+      <c r="D11" s="24"/>
       <c r="E11" s="24" t="s">
         <v>184</v>
       </c>
       <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="18" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="17" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="C12" s="24">
-        <v>25</v>
-      </c>
-      <c r="D12" s="24"/>
+        <v>0.109</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>195</v>
+      </c>
       <c r="E12" s="24" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="47"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="17" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C13" s="24">
+        <v>25</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="46"/>
+      <c r="B14" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="24">
         <v>0.3</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="47"/>
-      <c r="B14" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C14" s="41">
-        <v>0</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="18" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C15" s="24">
         <f>C19*(C43+C44+C45)*12/(10^6)</f>
@@ -2721,94 +2744,98 @@
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="38" t="s">
-        <v>235</v>
+      <c r="G15" s="37" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C16" s="24">
         <v>250</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C17" s="35">
         <v>250000</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C18" s="24">
         <v>1</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+      <c r="A19" s="41" t="s">
+        <v>254</v>
+      </c>
       <c r="B19" s="30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C19" s="24">
         <v>17</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="45" t="s">
         <v>176</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="C20" s="25">
-        <v>0.3</v>
+        <v>202</v>
+      </c>
+      <c r="C20" s="42">
+        <v>0</v>
       </c>
       <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
+      <c r="E20" s="25" t="s">
+        <v>200</v>
+      </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="46"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C21" s="39">
+        <v>240</v>
+      </c>
+      <c r="C21" s="38">
         <v>0.3</v>
       </c>
       <c r="D21" s="25"/>
@@ -2817,107 +2844,107 @@
       <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="45"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C22" s="27">
-        <f>C2*C16*C19*C8/(10^6)</f>
+        <f>C2*C16*C19*C9/(10^6)</f>
         <v>4517.75</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="27">
-        <f>C3*C17*C19*C8/(10^6)</f>
+        <f>C20*C17*C19*C9/(10^6)</f>
         <v>0</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="45"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" s="27">
-        <f>C4*C18*C19*1000*C8/(10^6)</f>
+        <f>C4*C18*C19*1000*C9/(10^6)</f>
         <v>903.55</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="45"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C25" s="32">
-        <f>C28*C13</f>
+        <f>C28*C14</f>
         <v>26666.666666666668</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="45"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C26" s="27">
-        <f>450*C8/1000</f>
-        <v>47.835000000000001</v>
+        <f>500*C9/1000</f>
+        <v>53.15</v>
       </c>
       <c r="D26" s="27"/>
       <c r="E26" s="27" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="45"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C27" s="27">
         <f>C26*C25/1000</f>
-        <v>1275.5999999999999</v>
+        <v>1417.3333333333333</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C28" s="32">
         <f>C5/0.45/10/200*10^6</f>
@@ -2925,36 +2952,36 @@
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="45"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C29" s="32">
-        <f>C5*C6/C7</f>
+        <f>C5*C6/C8</f>
         <v>54</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="45"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C30" s="32">
-        <f>C5/C7*1000*3600/C9/C10*C11/1000</f>
+        <f>C5/C8*1000*3600/C10/C11*C12/1000</f>
         <v>2053.375196232339</v>
       </c>
       <c r="D30" s="27"/>
@@ -2965,11 +2992,11 @@
       <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="43" t="s">
         <v>177</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C31" s="34">
         <f>SUM(C22:C24)</f>
@@ -2977,17 +3004,17 @@
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="44"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C32" s="34">
         <f>-C30</f>
@@ -2995,75 +3022,75 @@
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="44"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C33" s="34">
         <f>-C27</f>
-        <v>-1275.5999999999999</v>
+        <v>-1417.3333333333333</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="44"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C34" s="31">
-        <f>C31/C12</f>
+        <f>C31/C13</f>
         <v>216.852</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G34" s="20"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="44"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C35" s="42">
-        <f>-C29</f>
-        <v>-54</v>
+        <v>212</v>
+      </c>
+      <c r="C35" s="47">
+        <f>-C29/C7</f>
+        <v>-2.5592417061611375E-2</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G35" s="20"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B38" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -3074,15 +3101,15 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B42" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C43">
         <v>75000</v>
@@ -3090,7 +3117,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C44">
         <v>50000</v>
@@ -3098,7 +3125,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B45" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C45">
         <v>50000</v>

</xml_diff>

<commit_message>
Update of Ecopulpers and Database
The Main database has now the proper land category (Cropland) and CO2b are neglected since we don't fully understand their nature.
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Interventions/Biomass_ongrid.xlsx
+++ b/CVX_Kenya/Interventions/Biomass_ongrid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Interventions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6310E5E7-FC8C-4981-93D2-308607DA2608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DB64B7-8065-438A-9F15-EA21B809CA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="-10305" windowWidth="11070" windowHeight="5730" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -917,7 +917,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,6 +957,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,7 +1027,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1072,7 +1078,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1103,6 +1108,13 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1115,13 +1127,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1481,7 +1491,7 @@
       <c r="D2" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="32">
         <f>main!C35</f>
         <v>-2.5592417061611375E-2</v>
       </c>
@@ -1667,7 +1677,7 @@
       <c r="F3" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="39">
         <f>main!C33</f>
         <v>-1417.3333333333333</v>
       </c>
@@ -1774,7 +1784,7 @@
       <c r="E2" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="32">
         <f>main!C34</f>
         <v>216.852</v>
       </c>
@@ -2486,8 +2496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2525,7 +2535,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="17" t="s">
         <v>201</v>
       </c>
@@ -2540,11 +2550,11 @@
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="43">
         <f>C20</f>
         <v>0</v>
       </c>
@@ -2558,7 +2568,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="17" t="s">
         <v>203</v>
       </c>
@@ -2573,8 +2583,8 @@
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="36" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C5" s="24">
@@ -2590,11 +2600,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="36" t="s">
+      <c r="A6" s="48"/>
+      <c r="B6" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="38">
         <f>0.27</f>
         <v>0.27</v>
       </c>
@@ -2603,16 +2613,16 @@
         <v>243</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="36" t="s">
+      <c r="A7" s="48"/>
+      <c r="B7" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="38">
         <v>2110</v>
       </c>
       <c r="D7" s="24"/>
@@ -2620,12 +2630,12 @@
         <v>246</v>
       </c>
       <c r="F7" s="18"/>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="44" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="17" t="s">
         <v>207</v>
       </c>
@@ -2638,7 +2648,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="17" t="s">
         <v>210</v>
       </c>
@@ -2653,7 +2663,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="17" t="s">
         <v>179</v>
       </c>
@@ -2670,7 +2680,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="17" t="s">
         <v>181</v>
       </c>
@@ -2687,7 +2697,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="17" t="s">
         <v>182</v>
       </c>
@@ -2704,7 +2714,7 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="17" t="s">
         <v>213</v>
       </c>
@@ -2719,7 +2729,7 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="17" t="s">
         <v>221</v>
       </c>
@@ -2734,7 +2744,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="17" t="s">
         <v>234</v>
       </c>
@@ -2747,12 +2757,12 @@
         <v>188</v>
       </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="36" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="17" t="s">
         <v>230</v>
       </c>
@@ -2767,11 +2777,11 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="34">
         <v>250000</v>
       </c>
       <c r="D17" s="18"/>
@@ -2782,7 +2792,7 @@
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="17" t="s">
         <v>229</v>
       </c>
@@ -2797,30 +2807,30 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="50">
         <v>17</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24" t="s">
+      <c r="D19" s="50"/>
+      <c r="E19" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="47" t="s">
         <v>176</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="41">
         <v>0</v>
       </c>
       <c r="D20" s="25"/>
@@ -2831,11 +2841,11 @@
       <c r="G20" s="21"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="37">
         <v>0.3</v>
       </c>
       <c r="D21" s="25"/>
@@ -2844,7 +2854,7 @@
       <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="29" t="s">
         <v>198</v>
       </c>
@@ -2860,7 +2870,7 @@
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="44"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="29" t="s">
         <v>209</v>
       </c>
@@ -2876,7 +2886,7 @@
       <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="44"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="29" t="s">
         <v>199</v>
       </c>
@@ -2892,11 +2902,11 @@
       <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <f>C28*C14</f>
         <v>26666.666666666668</v>
       </c>
@@ -2908,7 +2918,7 @@
       <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="29" t="s">
         <v>224</v>
       </c>
@@ -2926,7 +2936,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="29" t="s">
         <v>225</v>
       </c>
@@ -2942,11 +2952,11 @@
       <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="44"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="31">
         <f>C5/0.45/10/200*10^6</f>
         <v>88888.888888888891</v>
       </c>
@@ -2960,11 +2970,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="44"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="31">
         <f>C5*C6/C8</f>
         <v>54</v>
       </c>
@@ -2976,11 +2986,11 @@
       <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="44"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="31">
         <f>C5/C8*1000*3600/C10/C11*C12/1000</f>
         <v>2053.375196232339</v>
       </c>
@@ -2992,13 +3002,13 @@
       <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="45" t="s">
         <v>177</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="33">
         <f>SUM(C22:C24)</f>
         <v>5421.3</v>
       </c>
@@ -3012,11 +3022,11 @@
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="34">
+      <c r="C32" s="33">
         <f>-C30</f>
         <v>-2053.375196232339</v>
       </c>
@@ -3030,11 +3040,11 @@
       <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="43"/>
+      <c r="A33" s="45"/>
       <c r="B33" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="33">
         <f>-C27</f>
         <v>-1417.3333333333333</v>
       </c>
@@ -3048,11 +3058,11 @@
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="43"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="C34" s="31">
+      <c r="C34" s="30">
         <f>C31/C13</f>
         <v>216.852</v>
       </c>
@@ -3066,11 +3076,11 @@
       <c r="G34" s="20"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="43"/>
+      <c r="A35" s="45"/>
       <c r="B35" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="C35" s="47">
+      <c r="C35" s="42">
         <f>-C29/C7</f>
         <v>-2.5592417061611375E-2</v>
       </c>

</xml_diff>